<commit_message>
add hours taken for sprint 1
</commit_message>
<xml_diff>
--- a/Burndown charts final.xlsx
+++ b/Burndown charts final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\IFB299\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidan\OneDrive\IFB299\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="72E0EB62C05BEC3327E557FECC79652E30545A61" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{9487CA31-1464-4993-A917-ED3079EB43F9}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="72E0EB62C05BEC3327E557FECC79652E30545A61" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{C9F826AF-74C2-484B-BD42-705B6F88CC32}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="2" r:id="rId1"/>
@@ -570,10 +570,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1070,7 +1070,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1154,10 +1154,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>25</c:v>
@@ -5474,16 +5474,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="29.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="29.85546875" style="1"/>
+    <col min="1" max="16384" width="29.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5503,27 +5503,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -5552,14 +5552,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>19</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>17</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -5743,17 +5743,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -5761,141 +5761,141 @@
         <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="2"/>
     </row>
-    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
     </row>
-    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
     </row>
   </sheetData>
@@ -5916,18 +5916,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5953,7 +5953,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -5981,7 +5981,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -6007,7 +6007,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -6022,7 +6022,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6031,7 +6031,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -6040,7 +6040,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6049,7 +6049,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -6060,7 +6060,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6075,7 +6075,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>19</v>
       </c>
@@ -6103,7 +6103,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18</v>
       </c>
@@ -6116,7 +6116,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>17</v>
       </c>
@@ -6129,7 +6129,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -6155,7 +6155,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -6168,7 +6168,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -6181,7 +6181,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -6194,7 +6194,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -6207,7 +6207,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10</v>
       </c>
@@ -6220,7 +6220,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -6233,7 +6233,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -6246,7 +6246,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -6259,7 +6259,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -6272,7 +6272,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5</v>
       </c>
@@ -6285,7 +6285,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -6298,7 +6298,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -6311,7 +6311,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -6337,7 +6337,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -6352,7 +6352,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -6361,7 +6361,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>

</xml_diff>